<commit_message>
update db and transactions
</commit_message>
<xml_diff>
--- a/DataBase/transactions.xlsx
+++ b/DataBase/transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub-Projects\ST_Python\Stock_Tracker\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{261E625E-5D8E-4127-AB79-64B58517E134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B66137-0590-4470-8864-C4ED22EBA8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{0CE267AD-AC6B-48BF-BB01-FB338060AAB0}"/>
+    <workbookView xWindow="-2160" yWindow="2580" windowWidth="21600" windowHeight="11835" xr2:uid="{0CE267AD-AC6B-48BF-BB01-FB338060AAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy Price </t>
+  </si>
+  <si>
+    <t>Sell Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>shark</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,12 +405,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7310C8-94F7-47B9-B855-61C67FA55F6C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>